<commit_message>
New data: Test 3
</commit_message>
<xml_diff>
--- a/ sgd.xlsx
+++ b/ sgd.xlsx
@@ -543,7 +543,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-1-5 15:55:35</t>
+          <t>2024-1-5 16:6:47</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -566,19 +566,19 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>15.7</v>
+        <v>15.6</v>
       </c>
       <c r="H2" t="n">
         <v>32</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1125</v>
+        <v>0.3468</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1125</v>
+        <v>0.309</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9203734020690376</v>
+        <v>0.9378940401964541</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>313.2</v>
+        <v>312.6</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
@@ -618,7 +618,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-1-5 15:55:38</t>
+          <t>2024-1-5 16:6:50</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -641,19 +641,19 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>15.7</v>
+        <v>15.6</v>
       </c>
       <c r="H3" t="n">
         <v>32</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0988</v>
+        <v>0.3346</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0988</v>
+        <v>0.3159</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9375805496534187</v>
+        <v>0.9330523529206869</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>313.8</v>
+        <v>312.9</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -693,7 +693,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-1-5 15:55:43</t>
+          <t>2024-1-5 16:6:55</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -716,19 +716,19 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>15.8</v>
+        <v>15.7</v>
       </c>
       <c r="H4" t="n">
         <v>32</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0993</v>
+        <v>0.3546</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0993</v>
+        <v>0.2919</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9221498484795708</v>
+        <v>0.9265038837995054</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>315.1</v>
+        <v>314.9</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
@@ -768,7 +768,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-1-5 15:55:46</t>
+          <t>2024-1-5 16:6:58</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -797,13 +797,13 @@
         <v>32</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3439</v>
+        <v>0.1616</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1995</v>
+        <v>0.1616</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9332961788986033</v>
+        <v>0.9331568497683653</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>315.7</v>
+        <v>315.1</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
@@ -843,7 +843,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-1-5 15:55:51</t>
+          <t>2024-1-5 16:7:3</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -866,19 +866,19 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>15.9</v>
+        <v>15.8</v>
       </c>
       <c r="H6" t="n">
         <v>32</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2458</v>
+        <v>0.3466</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2265</v>
+        <v>0.2541</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9459054651851336</v>
+        <v>0.9293252986868229</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="Q6" t="n">
-        <v>317.3</v>
+        <v>316.1</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
@@ -918,7 +918,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-1-5 15:55:55</t>
+          <t>2024-1-5 16:7:6</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -941,19 +941,19 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>15.9</v>
+        <v>15.8</v>
       </c>
       <c r="H7" t="n">
         <v>32</v>
       </c>
       <c r="I7" t="n">
-        <v>0.094</v>
+        <v>0.4458</v>
       </c>
       <c r="J7" t="n">
-        <v>0.094</v>
+        <v>0.2319</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9049775331777491</v>
+        <v>0.9424222369291859</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -977,7 +977,7 @@
         </is>
       </c>
       <c r="Q7" t="n">
-        <v>318</v>
+        <v>316.2</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
@@ -993,7 +993,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-1-5 15:55:55</t>
+          <t>2024-1-5 16:7:10</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1016,19 +1016,19 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>15.8</v>
+        <v>15.9</v>
       </c>
       <c r="H8" t="n">
         <v>32</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1901</v>
+        <v>0.1805</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1408</v>
+        <v>0.1283</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9398098157372252</v>
+        <v>0.9429795534501376</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>315.4</v>
+        <v>317.8</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
@@ -1068,7 +1068,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-1-5 15:56:1</t>
+          <t>2024-1-5 16:7:16</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1091,19 +1091,19 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>15.9</v>
+        <v>16</v>
       </c>
       <c r="H9" t="n">
         <v>32</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1901</v>
+        <v>0.4234</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1901</v>
+        <v>0.2026</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9365355811766345</v>
+        <v>0.934306315092828</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="Q9" t="n">
-        <v>317.9</v>
+        <v>319.9</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
@@ -1143,7 +1143,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-1-5 15:56:3</t>
+          <t>2024-1-5 16:7:16</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1166,19 +1166,19 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>15.8</v>
+        <v>15.9</v>
       </c>
       <c r="H10" t="n">
         <v>32</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2588</v>
+        <v>0.154</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2588</v>
+        <v>0.154</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9419345849733533</v>
+        <v>0.9265038837995054</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>316.5</v>
+        <v>317</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
@@ -1218,7 +1218,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-1-5 15:56:10</t>
+          <t>2024-1-5 16:7:22</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1247,13 +1247,13 @@
         <v>32</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2858</v>
+        <v>0.3563</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2624</v>
+        <v>0.0941</v>
       </c>
       <c r="K11" t="n">
-        <v>0.9345501410707444</v>
+        <v>0.9301612734682504</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>

</xml_diff>